<commit_message>
Hechos todos los requerimientos hasta RFC2
</commit_message>
<xml_diff>
--- a/Experimental/docs/Modelo Relacional AlohAndes.xlsx
+++ b/Experimental/docs/Modelo Relacional AlohAndes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Usuario\Desktop\Uniandes 2020-1\Sistrans\Sistrans\Experimental\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Juan\Documents\University\Sistemas Transaccionales\Sistrans\Experimental\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE95F77F-DD7D-482C-964F-F4AB04125060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F13C5B-0B6B-470E-9830-ADC0515F3491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="12900" xr2:uid="{F0CE3AD7-4FF2-4796-9B4F-1CAFCD41CF88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{F0CE3AD7-4FF2-4796-9B4F-1CAFCD41CF88}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
   <si>
     <t>AlohAndes</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>TipoEstablecimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -756,23 +759,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329E6558-AFF6-43EA-8345-4B4821A79FE3}">
   <dimension ref="B2:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="32.28515625" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="1" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="32.33203125" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -783,7 +786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -794,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -805,12 +808,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -833,7 +836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -856,7 +859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -873,13 +876,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -890,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -901,7 +904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -912,13 +915,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -950,7 +953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -982,7 +985,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -1014,12 +1017,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -1043,13 +1051,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -1097,12 +1105,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>41</v>
       </c>
@@ -1122,7 +1130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -1142,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>16</v>
       </c>
@@ -1156,12 +1164,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>22</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>5</v>
       </c>
@@ -1206,12 +1214,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>12</v>
       </c>
@@ -1222,7 +1230,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>4</v>
       </c>
@@ -1233,17 +1241,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>12</v>
       </c>
@@ -1251,7 +1259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>4</v>
       </c>
@@ -1259,7 +1267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>19</v>
       </c>
@@ -1267,12 +1275,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1288,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>19</v>
       </c>
@@ -1316,12 +1324,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100141F8B139A39EF4FBD26ECD02F5A5366" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="3a02e3438ac4a2584c0e2a34606e91e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="17da3363-7b33-4b13-9139-b2acfa28798a" xmlns:ns4="57bb2fa6-6ab7-49b8-a991-a3efc347c38f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33c97bc3b1320195e90d0b5eaf91005f" ns3:_="" ns4:_="">
     <xsd:import namespace="17da3363-7b33-4b13-9139-b2acfa28798a"/>
@@ -1492,6 +1494,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1502,23 +1510,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDDD124F-57B4-4374-8B01-05BC202C3053}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="57bb2fa6-6ab7-49b8-a991-a3efc347c38f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="17da3363-7b33-4b13-9139-b2acfa28798a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B30F7A1-82D8-47C3-BA13-3246471CDB9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1537,6 +1528,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDDD124F-57B4-4374-8B01-05BC202C3053}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="57bb2fa6-6ab7-49b8-a991-a3efc347c38f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="17da3363-7b33-4b13-9139-b2acfa28798a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B564E635-82B4-4ABA-930B-1062AC460E9D}">
   <ds:schemaRefs>

</xml_diff>